<commit_message>
CSA Table 10 Added
CSA Table 10 has been added and formatted
</commit_message>
<xml_diff>
--- a/AEUC_CSA_clearances.xlsx
+++ b/AEUC_CSA_clearances.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="141" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DE7F065-E9B7-4496-AF72-2091206F5530}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-6855" windowWidth="16440" windowHeight="28440" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AEUC Table 5" sheetId="1" r:id="rId1"/>
@@ -14720,8 +14720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984872E1-D2BB-4B10-9448-113DF36AF448}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added CSA table 11
CSA table added and working
</commit_message>
<xml_diff>
--- a/AEUC_CSA_clearances.xlsx
+++ b/AEUC_CSA_clearances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://powereng0-my.sharepoint.com/personal/yeh-in_kang_powereng_com/Documents/Desktop/Python Stuff/Clearance Calcs/CSA-clearances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DE7F065-E9B7-4496-AF72-2091206F5530}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EAC427D-4833-435A-BC5B-CD6B87767B27}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-6855" windowWidth="16440" windowHeight="28440" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AEUC Table 5" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,8 @@
     <sheet name="CSA table 6" sheetId="9" r:id="rId8"/>
     <sheet name="CSA table 7" sheetId="10" r:id="rId9"/>
     <sheet name="CSA table 9" sheetId="11" r:id="rId10"/>
-    <sheet name="CSA table 10" sheetId="12" r:id="rId11"/>
-    <sheet name="CSA table 11" sheetId="13" r:id="rId12"/>
+    <sheet name="CSA table 11" sheetId="13" r:id="rId11"/>
+    <sheet name="CSA table 10" sheetId="12" r:id="rId12"/>
     <sheet name="CSA table 13" sheetId="14" r:id="rId13"/>
     <sheet name="CSA table 14" sheetId="15" r:id="rId14"/>
     <sheet name="CSA table 15" sheetId="16" r:id="rId15"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4305" uniqueCount="1660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4318" uniqueCount="1673">
   <si>
     <t>Location of Wires or Conductors</t>
   </si>
@@ -5105,6 +5105,45 @@
   </si>
   <si>
     <t>Inaccessible Conductor not Attached Under Bridge (Vertical)</t>
+  </si>
+  <si>
+    <t>Equipment or Conductors</t>
+  </si>
+  <si>
+    <t>Supply equipment</t>
+  </si>
+  <si>
+    <t>Guys, messengers, span wires, communication circuits, secondary cable 0–750 V, and multi-grounded neutral conductors</t>
+  </si>
+  <si>
+    <t>Other supply conductors ≤ 22kV</t>
+  </si>
+  <si>
+    <t>Supply conductors &gt; 150 kV</t>
+  </si>
+  <si>
+    <t>A — Measured in any direction from the water level, edge of pool, or diving platform</t>
+  </si>
+  <si>
+    <t>B — Measured vertically over land</t>
+  </si>
+  <si>
+    <t>Supply conductors &gt; 22 kV and ≤ 150 kV (6.7 + 0.01 m/kV above 22kV)</t>
+  </si>
+  <si>
+    <t>See Clause 5.3.2 and Table 5</t>
+  </si>
+  <si>
+    <t>See Clause 5.3.1 and Table 2 and Table 4</t>
+  </si>
+  <si>
+    <t>See Clause 5.3.1 and Table 2 and Table 5</t>
+  </si>
+  <si>
+    <t>See Clause 5.3.1 and Table 2 and Table 6</t>
+  </si>
+  <si>
+    <t>See Clause 5.3.1 and Table 2 and Table 7</t>
   </si>
 </sst>
 </file>
@@ -14717,10 +14756,97 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98AFE7E7-CAAC-400D-838A-9F5291087BA6}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
+        <v>1660</v>
+      </c>
+      <c r="B1" s="70" t="s">
+        <v>1665</v>
+      </c>
+      <c r="C1" s="70" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="70" t="s">
+        <v>1661</v>
+      </c>
+      <c r="B2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="70" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="70" t="s">
+        <v>1663</v>
+      </c>
+      <c r="B4">
+        <v>6.7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="70" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B5">
+        <v>6.7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="70" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984872E1-D2BB-4B10-9448-113DF36AF448}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:L5"/>
     </sheetView>
   </sheetViews>
@@ -14988,18 +15114,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98AFE7E7-CAAC-400D-838A-9F5291087BA6}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
CSA Table 13 added
Added CSA table 13
</commit_message>
<xml_diff>
--- a/AEUC_CSA_clearances.xlsx
+++ b/AEUC_CSA_clearances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://powereng0-my.sharepoint.com/personal/yeh-in_kang_powereng_com/Documents/Desktop/Python Stuff/Clearance Calcs/CSA-clearances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EAC427D-4833-435A-BC5B-CD6B87767B27}"/>
+  <xr:revisionPtr revIDLastSave="334" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6774E9BF-6913-4096-A3D0-C10668C06654}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AEUC Table 5" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,8 @@
     <sheet name="CSA table 6" sheetId="9" r:id="rId8"/>
     <sheet name="CSA table 7" sheetId="10" r:id="rId9"/>
     <sheet name="CSA table 9" sheetId="11" r:id="rId10"/>
-    <sheet name="CSA table 11" sheetId="13" r:id="rId11"/>
-    <sheet name="CSA table 10" sheetId="12" r:id="rId12"/>
+    <sheet name="CSA table 10" sheetId="12" r:id="rId11"/>
+    <sheet name="CSA table 11" sheetId="13" r:id="rId12"/>
     <sheet name="CSA table 13" sheetId="14" r:id="rId13"/>
     <sheet name="CSA table 14" sheetId="15" r:id="rId14"/>
     <sheet name="CSA table 15" sheetId="16" r:id="rId15"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4318" uniqueCount="1673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4342" uniqueCount="1687">
   <si>
     <t>Location of Wires or Conductors</t>
   </si>
@@ -5144,6 +5144,48 @@
   </si>
   <si>
     <t>See Clause 5.3.1 and Table 2 and Table 7</t>
+  </si>
+  <si>
+    <t>Type of line wire, cable, or other plant being crossed over</t>
+  </si>
+  <si>
+    <t>Communication wires and cables</t>
+  </si>
+  <si>
+    <t>AC 0-0.75</t>
+  </si>
+  <si>
+    <t>AC &lt; 0.75 ≤ 22</t>
+  </si>
+  <si>
+    <t>AC &lt; 22 ≤ 50</t>
+  </si>
+  <si>
+    <t>AC &lt; 50 ≤ 90</t>
+  </si>
+  <si>
+    <t>AC &lt; 90 ≤ 120</t>
+  </si>
+  <si>
+    <t>AC &lt; 120 ≤ 150</t>
+  </si>
+  <si>
+    <t>AC &lt; 150 ≤ 190</t>
+  </si>
+  <si>
+    <t>AC &lt; 190 ≤ 220</t>
+  </si>
+  <si>
+    <t>AC &lt; 220 ≤ 320</t>
+  </si>
+  <si>
+    <t>AC &lt; 320 ≤ 425</t>
+  </si>
+  <si>
+    <t>Guys, span wires, and aerial grounding wires</t>
+  </si>
+  <si>
+    <t>Guys, span wires, aerial grounding conductors, and communication wires and cables</t>
   </si>
 </sst>
 </file>
@@ -14756,93 +14798,6 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98AFE7E7-CAAC-400D-838A-9F5291087BA6}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
-        <v>1660</v>
-      </c>
-      <c r="B1" s="70" t="s">
-        <v>1665</v>
-      </c>
-      <c r="C1" s="70" t="s">
-        <v>1666</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="s">
-        <v>1661</v>
-      </c>
-      <c r="B2">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1668</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="70" t="s">
-        <v>1662</v>
-      </c>
-      <c r="B3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1669</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="70" t="s">
-        <v>1663</v>
-      </c>
-      <c r="B4">
-        <v>6.7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1670</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="70" t="s">
-        <v>1667</v>
-      </c>
-      <c r="B5">
-        <v>6.7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>1671</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
-        <v>1664</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>1672</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984872E1-D2BB-4B10-9448-113DF36AF448}">
   <dimension ref="A1:M6"/>
   <sheetViews>
@@ -15118,14 +15073,455 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98AFE7E7-CAAC-400D-838A-9F5291087BA6}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
+        <v>1660</v>
+      </c>
+      <c r="B1" s="70" t="s">
+        <v>1665</v>
+      </c>
+      <c r="C1" s="70" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="70" t="s">
+        <v>1661</v>
+      </c>
+      <c r="B2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="70" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="70" t="s">
+        <v>1663</v>
+      </c>
+      <c r="B4">
+        <v>6.7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="70" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B5">
+        <v>6.7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="70" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD4E87C-FFE6-4F04-88CA-B35A47E7587C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1"/>
+    <col min="11" max="12" width="13.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1686</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1675</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1676</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1677</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1678</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1679</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1680</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1682</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1683</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B2">
+        <v>0.2</v>
+      </c>
+      <c r="C2">
+        <v>0.3</v>
+      </c>
+      <c r="D2">
+        <v>0.6</v>
+      </c>
+      <c r="E2">
+        <v>0.9</v>
+      </c>
+      <c r="F2">
+        <v>1.2</v>
+      </c>
+      <c r="G2">
+        <v>1.5</v>
+      </c>
+      <c r="H2">
+        <v>1.8</v>
+      </c>
+      <c r="I2">
+        <v>2.4</v>
+      </c>
+      <c r="J2">
+        <v>2.7</v>
+      </c>
+      <c r="K2">
+        <v>3.9</v>
+      </c>
+      <c r="L2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C3">
+        <v>0.3</v>
+      </c>
+      <c r="D3">
+        <v>0.3</v>
+      </c>
+      <c r="E3">
+        <v>0.7</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1.2</v>
+      </c>
+      <c r="H3">
+        <v>1.6</v>
+      </c>
+      <c r="I3">
+        <v>2.1</v>
+      </c>
+      <c r="J3">
+        <v>2.6</v>
+      </c>
+      <c r="K3">
+        <v>3.7</v>
+      </c>
+      <c r="L3">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1676</v>
+      </c>
+      <c r="C4">
+        <v>0.3</v>
+      </c>
+      <c r="D4">
+        <v>0.4</v>
+      </c>
+      <c r="E4">
+        <v>0.8</v>
+      </c>
+      <c r="F4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G4">
+        <v>1.3</v>
+      </c>
+      <c r="H4">
+        <v>1.7</v>
+      </c>
+      <c r="I4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J4">
+        <v>2.7</v>
+      </c>
+      <c r="K4">
+        <v>3.8</v>
+      </c>
+      <c r="L4">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C5">
+        <v>0.7</v>
+      </c>
+      <c r="D5">
+        <v>0.8</v>
+      </c>
+      <c r="E5">
+        <v>0.9</v>
+      </c>
+      <c r="F5">
+        <v>1.2</v>
+      </c>
+      <c r="G5">
+        <v>1.4</v>
+      </c>
+      <c r="H5">
+        <v>1.9</v>
+      </c>
+      <c r="I5">
+        <v>2.4</v>
+      </c>
+      <c r="J5">
+        <v>2.8</v>
+      </c>
+      <c r="K5">
+        <v>3.9</v>
+      </c>
+      <c r="L5">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1678</v>
+      </c>
+      <c r="F6">
+        <v>1.3</v>
+      </c>
+      <c r="G6">
+        <v>1.6</v>
+      </c>
+      <c r="H6">
+        <v>2.1</v>
+      </c>
+      <c r="I6">
+        <v>2.6</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="L6">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1679</v>
+      </c>
+      <c r="G7">
+        <v>1.8</v>
+      </c>
+      <c r="H7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I7">
+        <v>2.8</v>
+      </c>
+      <c r="J7">
+        <v>3.2</v>
+      </c>
+      <c r="K7">
+        <v>4.3</v>
+      </c>
+      <c r="L7">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1680</v>
+      </c>
+      <c r="H8">
+        <v>2.4</v>
+      </c>
+      <c r="I8">
+        <v>2.9</v>
+      </c>
+      <c r="J8">
+        <v>3.4</v>
+      </c>
+      <c r="K8">
+        <v>4.5</v>
+      </c>
+      <c r="L8">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1681</v>
+      </c>
+      <c r="I9">
+        <v>3.2</v>
+      </c>
+      <c r="J9">
+        <v>3.6</v>
+      </c>
+      <c r="K9">
+        <v>4.7</v>
+      </c>
+      <c r="L9">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1682</v>
+      </c>
+      <c r="J10">
+        <v>3.7</v>
+      </c>
+      <c r="K10">
+        <v>4.8</v>
+      </c>
+      <c r="L10">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1683</v>
+      </c>
+      <c r="K11">
+        <v>5.4</v>
+      </c>
+      <c r="L11">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1684</v>
+      </c>
+      <c r="L12">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B13">
+        <v>0.2</v>
+      </c>
+      <c r="C13">
+        <v>0.2</v>
+      </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+      <c r="E13">
+        <v>0.8</v>
+      </c>
+      <c r="F13">
+        <v>1.2</v>
+      </c>
+      <c r="G13">
+        <v>1.5</v>
+      </c>
+      <c r="H13">
+        <v>1.8</v>
+      </c>
+      <c r="I13">
+        <v>2.4</v>
+      </c>
+      <c r="J13">
+        <v>2.7</v>
+      </c>
+      <c r="K13">
+        <v>3.4</v>
+      </c>
+      <c r="L13">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
CSA 14 table added
CSA 14 clearance table added
</commit_message>
<xml_diff>
--- a/AEUC_CSA_clearances.xlsx
+++ b/AEUC_CSA_clearances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://powereng0-my.sharepoint.com/personal/yeh-in_kang_powereng_com/Documents/Desktop/Python Stuff/Clearance Calcs/CSA-clearances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="334" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6774E9BF-6913-4096-A3D0-C10668C06654}"/>
+  <xr:revisionPtr revIDLastSave="384" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF8AA127-E657-4B73-8EDA-4599879AC533}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AEUC Table 5" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4342" uniqueCount="1687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4356" uniqueCount="1698">
   <si>
     <t>Location of Wires or Conductors</t>
   </si>
@@ -5186,6 +5186,39 @@
   </si>
   <si>
     <t>Guys, span wires, aerial grounding conductors, and communication wires and cables</t>
+  </si>
+  <si>
+    <t>0 – 750V</t>
+  </si>
+  <si>
+    <t>&gt;90kV&lt;120kV</t>
+  </si>
+  <si>
+    <t>&gt;120kV&lt;150kV</t>
+  </si>
+  <si>
+    <t>&gt;150kV&lt;190kV</t>
+  </si>
+  <si>
+    <t>&gt;190kV&lt;220kV</t>
+  </si>
+  <si>
+    <t>&gt;220kV&lt;320kV</t>
+  </si>
+  <si>
+    <t>&gt;320kV&lt;425kV</t>
+  </si>
+  <si>
+    <t>Communication conductors and cables, span and grounding wires carried aerially</t>
+  </si>
+  <si>
+    <t>Type of plant being crossed over</t>
+  </si>
+  <si>
+    <t>Aerial tramways Gondolas and similar apparatus providing a roof over passengers</t>
+  </si>
+  <si>
+    <t>Chairlifts, T-bars, and similar apparatus or towers of any type of aerial tramway</t>
   </si>
 </sst>
 </file>
@@ -15164,7 +15197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD4E87C-FFE6-4F04-88CA-B35A47E7587C}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -15528,13 +15561,136 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1483A29D-C531-4BC7-B282-D7E221D1D550}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1694</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1687</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1544</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1545</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1546</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1688</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1692</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B2">
+        <v>0.15</v>
+      </c>
+      <c r="C2">
+        <v>0.15</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>0.8</v>
+      </c>
+      <c r="F2">
+        <v>1.2</v>
+      </c>
+      <c r="G2">
+        <v>1.5</v>
+      </c>
+      <c r="H2">
+        <v>1.8</v>
+      </c>
+      <c r="I2">
+        <v>2.4</v>
+      </c>
+      <c r="J2">
+        <v>2.7</v>
+      </c>
+      <c r="K2">
+        <v>3.9</v>
+      </c>
+      <c r="L2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1697</v>
+      </c>
+      <c r="B3">
+        <v>1.7</v>
+      </c>
+      <c r="C3">
+        <v>1.7</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F3">
+        <v>2.7</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>3.4</v>
+      </c>
+      <c r="I3">
+        <v>3.9</v>
+      </c>
+      <c r="J3">
+        <v>4.3</v>
+      </c>
+      <c r="K3">
+        <v>5.4</v>
+      </c>
+      <c r="L3">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added CSA table 15 and 16
CSA table 15 will need review have no clue how the communication numbers were found on the CSA spreadsheet
</commit_message>
<xml_diff>
--- a/AEUC_CSA_clearances.xlsx
+++ b/AEUC_CSA_clearances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://powereng0-my.sharepoint.com/personal/yeh-in_kang_powereng_com/Documents/Desktop/Python Stuff/Clearance Calcs/CSA-clearances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="384" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF8AA127-E657-4B73-8EDA-4599879AC533}"/>
+  <xr:revisionPtr revIDLastSave="427" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5EC4702-EACA-40A8-94FE-16418A29E56C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AEUC Table 5" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4356" uniqueCount="1698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4367" uniqueCount="1709">
   <si>
     <t>Location of Wires or Conductors</t>
   </si>
@@ -5219,6 +5219,39 @@
   </si>
   <si>
     <t>Chairlifts, T-bars, and similar apparatus or towers of any type of aerial tramway</t>
+  </si>
+  <si>
+    <t>Sum of voltages of conductors</t>
+  </si>
+  <si>
+    <t>0-750V</t>
+  </si>
+  <si>
+    <t>Clearance increment (mm)</t>
+  </si>
+  <si>
+    <t>&gt; 750 V ac (300 + 10 mm/kV over 750)</t>
+  </si>
+  <si>
+    <t>Voltage of line conductor</t>
+  </si>
+  <si>
+    <t>&gt;22 &lt; 50</t>
+  </si>
+  <si>
+    <t>&gt;50 (+10mm/kV over 50kV)</t>
+  </si>
+  <si>
+    <t>&gt; 5 &lt; 22 (1000 wherever practicable, but in no case less than 500)</t>
+  </si>
+  <si>
+    <t>Clearance increment, mm</t>
+  </si>
+  <si>
+    <t>&gt; 750 V dc (300 + 6 mm/kV over 750)</t>
+  </si>
+  <si>
+    <t>0-5 (1000 where practicable, but in no case less than. a)150 for spans 0-6m b)230 for spans &gt;6 and &lt; 15m c)300 for spans &gt;15m</t>
   </si>
 </sst>
 </file>
@@ -15563,7 +15596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1483A29D-C531-4BC7-B282-D7E221D1D550}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
@@ -15696,24 +15729,110 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D291676-B421-4732-AE26-3C83CCB2E396}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1701</v>
+      </c>
+      <c r="B3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE21A4C-EC48-40A7-A901-B56AB1FC4A39}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.21875" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1708</v>
+      </c>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="B3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>1703</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B5">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
CSA table 17 added
CSA table 17 has been added to the script
</commit_message>
<xml_diff>
--- a/AEUC_CSA_clearances.xlsx
+++ b/AEUC_CSA_clearances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://powereng0-my.sharepoint.com/personal/yeh-in_kang_powereng_com/Documents/Desktop/Python Stuff/Clearance Calcs/CSA-clearances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="427" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5EC4702-EACA-40A8-94FE-16418A29E56C}"/>
+  <xr:revisionPtr revIDLastSave="465" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92E93A37-C719-4351-8B55-4DD64496FB07}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-10920" windowWidth="16440" windowHeight="28440" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AEUC Table 5" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,9 @@
     <sheet name="CSA table 11" sheetId="13" r:id="rId12"/>
     <sheet name="CSA table 13" sheetId="14" r:id="rId13"/>
     <sheet name="CSA table 14" sheetId="15" r:id="rId14"/>
-    <sheet name="CSA table 15" sheetId="16" r:id="rId15"/>
-    <sheet name="CSA table 16" sheetId="17" r:id="rId16"/>
-    <sheet name="CSA table 17" sheetId="18" r:id="rId17"/>
+    <sheet name="CSA table 17" sheetId="18" r:id="rId15"/>
+    <sheet name="CSA table 15" sheetId="16" r:id="rId16"/>
+    <sheet name="CSA table 16" sheetId="17" r:id="rId17"/>
     <sheet name="CSA table 18" sheetId="19" r:id="rId18"/>
     <sheet name="CSA table 20" sheetId="20" r:id="rId19"/>
     <sheet name="CSA table 21" sheetId="21" r:id="rId20"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4367" uniqueCount="1709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4374" uniqueCount="1716">
   <si>
     <t>Location of Wires or Conductors</t>
   </si>
@@ -5252,6 +5252,27 @@
   </si>
   <si>
     <t>0-5 (1000 where practicable, but in no case less than. a)150 for spans 0-6m b)230 for spans &gt;6 and &lt; 15m c)300 for spans &gt;15m</t>
+  </si>
+  <si>
+    <t>Line conductor</t>
+  </si>
+  <si>
+    <t>0-5 kV ac &gt; 6 &lt; 50 m</t>
+  </si>
+  <si>
+    <t>0-5 kV ac 0 - 6 m</t>
+  </si>
+  <si>
+    <t>Minimum seperation(mm)</t>
+  </si>
+  <si>
+    <t>&gt; 5kV ac &lt; 50 m + 10 mm/kV over 1kV</t>
+  </si>
+  <si>
+    <t>0-5 kV ac  &gt; 50 &lt; 450 m a )3 x the distance (in m) by which the span length exceeds 50 m; b)83 x the final unloaded sag (in m) at 15C conductor temperature for conductor(s) having the greatest sag; and c)10 mm/kV over 5 kV.</t>
+  </si>
+  <si>
+    <t>&gt; 5kV ac &gt; 50 &lt; 450 m a )3 x the distance (in m) by which the span length exceeds 50 m; b)83 x the final unloaded sag (in m) at 15C conductor temperature for conductor(s) having the greatest sag; and c)10 mm/kV over 5 kV.</t>
   </si>
 </sst>
 </file>
@@ -15728,6 +15749,74 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223DF239-8478-497B-8099-A6F4F5B834F8}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="69" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B6">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D291676-B421-4732-AE26-3C83CCB2E396}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -15778,11 +15867,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE21A4C-EC48-40A7-A901-B56AB1FC4A39}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -15833,18 +15922,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223DF239-8478-497B-8099-A6F4F5B834F8}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added up to CSA table 20
done up to CSA table 20
</commit_message>
<xml_diff>
--- a/AEUC_CSA_clearances.xlsx
+++ b/AEUC_CSA_clearances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://powereng0-my.sharepoint.com/personal/yeh-in_kang_powereng_com/Documents/Desktop/Python Stuff/Clearance Calcs/CSA-clearances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="465" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92E93A37-C719-4351-8B55-4DD64496FB07}"/>
+  <xr:revisionPtr revIDLastSave="574" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE0CFF4D-3C58-4BE8-8262-331AE3897420}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-10920" windowWidth="16440" windowHeight="28440" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="18" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AEUC Table 5" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,9 @@
     <sheet name="CSA table 11" sheetId="13" r:id="rId12"/>
     <sheet name="CSA table 13" sheetId="14" r:id="rId13"/>
     <sheet name="CSA table 14" sheetId="15" r:id="rId14"/>
-    <sheet name="CSA table 17" sheetId="18" r:id="rId15"/>
-    <sheet name="CSA table 15" sheetId="16" r:id="rId16"/>
-    <sheet name="CSA table 16" sheetId="17" r:id="rId17"/>
+    <sheet name="CSA table 15" sheetId="16" r:id="rId15"/>
+    <sheet name="CSA table 16" sheetId="17" r:id="rId16"/>
+    <sheet name="CSA table 17" sheetId="18" r:id="rId17"/>
     <sheet name="CSA table 18" sheetId="19" r:id="rId18"/>
     <sheet name="CSA table 20" sheetId="20" r:id="rId19"/>
     <sheet name="CSA table 21" sheetId="21" r:id="rId20"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4374" uniqueCount="1716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4395" uniqueCount="1732">
   <si>
     <t>Location of Wires or Conductors</t>
   </si>
@@ -5273,6 +5273,54 @@
   </si>
   <si>
     <t>&gt; 5kV ac &gt; 50 &lt; 450 m a )3 x the distance (in m) by which the span length exceeds 50 m; b)83 x the final unloaded sag (in m) at 15C conductor temperature for conductor(s) having the greatest sag; and c)10 mm/kV over 5 kV.</t>
+  </si>
+  <si>
+    <t>Conductors at lower level</t>
+  </si>
+  <si>
+    <t>AC 0-750 V</t>
+  </si>
+  <si>
+    <t>AC &gt; 5 ≤ 22</t>
+  </si>
+  <si>
+    <t>AC &gt; 0.75 ≤ 5</t>
+  </si>
+  <si>
+    <t>AC &gt; 22 ≤ 50</t>
+  </si>
+  <si>
+    <t>AC &gt; 50 ≤ 90</t>
+  </si>
+  <si>
+    <t>Between circuit conductors</t>
+  </si>
+  <si>
+    <t>Maximum circuit line-to-ground voltage, kV</t>
+  </si>
+  <si>
+    <t>Between multi-grounded neutral and circuit conductor</t>
+  </si>
+  <si>
+    <t>0.75 kV</t>
+  </si>
+  <si>
+    <t>5 kV</t>
+  </si>
+  <si>
+    <t>10 kV</t>
+  </si>
+  <si>
+    <t>15 kV</t>
+  </si>
+  <si>
+    <t>22 kV</t>
+  </si>
+  <si>
+    <t>50 kV</t>
+  </si>
+  <si>
+    <t>90 kV</t>
   </si>
 </sst>
 </file>
@@ -15252,7 +15300,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection sqref="A1:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15749,74 +15797,6 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223DF239-8478-497B-8099-A6F4F5B834F8}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="34.109375" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
-        <v>1709</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>1712</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1711</v>
-      </c>
-      <c r="B2">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1710</v>
-      </c>
-      <c r="B3">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>1714</v>
-      </c>
-      <c r="B4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>1713</v>
-      </c>
-      <c r="B5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>1715</v>
-      </c>
-      <c r="B6">
-        <v>300</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D291676-B421-4732-AE26-3C83CCB2E396}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -15867,7 +15847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE21A4C-EC48-40A7-A901-B56AB1FC4A39}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -15926,26 +15906,314 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223DF239-8478-497B-8099-A6F4F5B834F8}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="69" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B6">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEDF121-3F1D-4C33-B24A-FF0D03551444}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" customWidth="1"/>
+    <col min="7" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1717</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1719</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1718</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B2">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
+        <v>0.4</v>
+      </c>
+      <c r="D2">
+        <v>0.4</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1719</v>
+      </c>
+      <c r="C3">
+        <v>0.4</v>
+      </c>
+      <c r="D3">
+        <v>0.4</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1718</v>
+      </c>
+      <c r="D4">
+        <v>0.4</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1721</v>
+      </c>
+      <c r="F6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F855B213-C4DE-4094-9F76-E7B35D3988F6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B3">
+        <v>150</v>
+      </c>
+      <c r="C3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B4">
+        <v>150</v>
+      </c>
+      <c r="C4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B5">
+        <v>250</v>
+      </c>
+      <c r="C5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B6">
+        <v>350</v>
+      </c>
+      <c r="C6">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B7">
+        <v>750</v>
+      </c>
+      <c r="C7">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B8">
+        <v>1000</v>
+      </c>
+      <c r="C8">
+        <v>1250</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
CSA table 22 code made
Made python code for sorting through text and only changing numbers in that text, it could be useful in the future
</commit_message>
<xml_diff>
--- a/AEUC_CSA_clearances.xlsx
+++ b/AEUC_CSA_clearances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://powereng0-my.sharepoint.com/personal/yeh-in_kang_powereng_com/Documents/Desktop/Python Stuff/Clearance Calcs/CSA-clearances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="801" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41467337-2EE3-4219-88BF-795E0D96E9E1}"/>
+  <xr:revisionPtr revIDLastSave="828" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BC6F224-2021-44D9-A955-F7D278E897DF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="18" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57600" yWindow="-6735" windowWidth="16200" windowHeight="9390" firstSheet="18" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AEUC Table 5" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4465" uniqueCount="1781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4480" uniqueCount="1792">
   <si>
     <t>Location of Wires or Conductors</t>
   </si>
@@ -5469,12 +5469,45 @@
   <si>
     <t>&gt; 22 kV (+10mm/kV over 22kV)</t>
   </si>
+  <si>
+    <t>75**</t>
+  </si>
+  <si>
+    <t>§§</t>
+  </si>
+  <si>
+    <t>170††‡‡</t>
+  </si>
+  <si>
+    <t>100††</t>
+  </si>
+  <si>
+    <t>To best eng practice, but no less than 917 mm</t>
+  </si>
+  <si>
+    <t>To best eng practice, but no less than 767 mm</t>
+  </si>
+  <si>
+    <t>To best eng practice, but no less than 997 mm</t>
+  </si>
+  <si>
+    <t>300‡</t>
+  </si>
+  <si>
+    <t>150‡</t>
+  </si>
+  <si>
+    <t>380‡††</t>
+  </si>
+  <si>
+    <t>&gt; 50 kV</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5574,6 +5607,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -6428,7 +6467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6754,6 +6793,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16529,7 +16569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53C1BD1-0BC0-4032-A11F-606EC57A209E}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -16716,18 +16756,19 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDDF029-148A-4983-A864-F18C1F696E3E}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="70" t="s">
         <v>1741</v>
       </c>
@@ -16743,8 +16784,11 @@
       <c r="E1" s="70" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F1" s="70" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="70" t="s">
         <v>1742</v>
       </c>
@@ -16757,13 +16801,19 @@
       <c r="D2">
         <v>300</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E2" s="119" t="s">
+        <v>1788</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="70" t="s">
         <v>1743</v>
       </c>
-      <c r="B3">
-        <v>75</v>
+      <c r="B3" t="s">
+        <v>1781</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -16771,24 +16821,51 @@
       <c r="D3">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="70" t="s">
         <v>1744</v>
       </c>
-      <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="C4">
-        <v>170</v>
+      <c r="B4" t="s">
+        <v>1784</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1783</v>
       </c>
       <c r="D4">
         <v>380</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>1790</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="70" t="s">
         <v>1745</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1782</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1782</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1782</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1782</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done CSA table 26
Now have code for all tables. Only thing left to do is to review as well as look at tables 18, 21, and 15
</commit_message>
<xml_diff>
--- a/AEUC_CSA_clearances.xlsx
+++ b/AEUC_CSA_clearances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://powereng0-my.sharepoint.com/personal/yeh-in_kang_powereng_com/Documents/Desktop/Python Stuff/Clearance Calcs/CSA-clearances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="848" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3F2D02E-1F24-4904-9785-277A2EB67857}"/>
+  <xr:revisionPtr revIDLastSave="851" documentId="13_ncr:1_{8395011A-BAF9-4565-AFF6-31B2472E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2C7BF8A-0444-40E4-9545-DAFB66007631}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="21" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="20" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AEUC Table 5" sheetId="1" r:id="rId1"/>
@@ -34,11 +34,11 @@
     <sheet name="CSA table 20" sheetId="20" r:id="rId19"/>
     <sheet name="CSA table 21" sheetId="21" r:id="rId20"/>
     <sheet name="CSA table 22" sheetId="22" r:id="rId21"/>
-    <sheet name="CSA table 23" sheetId="23" r:id="rId22"/>
-    <sheet name="CSA table 24" sheetId="24" r:id="rId23"/>
-    <sheet name="CSA table 25" sheetId="25" r:id="rId24"/>
-    <sheet name="CSA table 26" sheetId="26" r:id="rId25"/>
-    <sheet name="CSA C22.3 No.1 Table D2" sheetId="27" r:id="rId26"/>
+    <sheet name="CSA C22.3 No.1 Table D2" sheetId="27" r:id="rId22"/>
+    <sheet name="CSA table 23" sheetId="23" r:id="rId23"/>
+    <sheet name="CSA table 24" sheetId="24" r:id="rId24"/>
+    <sheet name="CSA table 25" sheetId="25" r:id="rId25"/>
+    <sheet name="CSA table 26" sheetId="26" r:id="rId26"/>
     <sheet name="CSA C22.3 No.60826 Table CA.1" sheetId="28" r:id="rId27"/>
   </sheets>
   <externalReferences>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4487" uniqueCount="1797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4489" uniqueCount="1798">
   <si>
     <t>Location of Wires or Conductors</t>
   </si>
@@ -5516,6 +5516,9 @@
   </si>
   <si>
     <t>75*†</t>
+  </si>
+  <si>
+    <t>150*</t>
   </si>
 </sst>
 </file>
@@ -16889,402 +16892,6 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4407B8D6-4BCD-4778-A70E-F76356A6ED49}">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
-        <v>1741</v>
-      </c>
-      <c r="B1" s="70" t="s">
-        <v>1746</v>
-      </c>
-      <c r="C1" s="70" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="70" t="s">
-        <v>1795</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="s">
-        <v>1749</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1791</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1793</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1794</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="70" t="s">
-        <v>1753</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1791</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="70" t="s">
-        <v>1754</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1792</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1792</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="70" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B5">
-        <v>0.75</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
-        <v>1756</v>
-      </c>
-      <c r="B6">
-        <v>0.1</v>
-      </c>
-      <c r="C6">
-        <v>0.3</v>
-      </c>
-      <c r="D6">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="70" t="s">
-        <v>1750</v>
-      </c>
-      <c r="B7">
-        <v>0.3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1757</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="70" t="s">
-        <v>1759</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="70" t="s">
-        <v>1758</v>
-      </c>
-      <c r="B9">
-        <v>0.1</v>
-      </c>
-      <c r="C9">
-        <v>0.1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="70" t="s">
-        <v>1751</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1791</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1757</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="70" t="s">
-        <v>1752</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1757</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1757</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7AF96B-9516-4E8F-906F-2D6A1CFA8D27}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="36.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1764</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1761</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1796</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1762</v>
-      </c>
-      <c r="B3">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>1763</v>
-      </c>
-      <c r="B4">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>1765</v>
-      </c>
-      <c r="B5">
-        <v>380</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DBE3240-1F9D-4EBB-8E6B-063E85AF465C}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1766</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1767</v>
-      </c>
-      <c r="B2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1770</v>
-      </c>
-      <c r="B3">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>1769</v>
-      </c>
-      <c r="B4">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>1772</v>
-      </c>
-      <c r="B5">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>1768</v>
-      </c>
-      <c r="B6">
-        <v>0.6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D87E58B-D1A3-4FBD-9C66-ABF5F5BF1B0C}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1773</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1777</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1778</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1767</v>
-      </c>
-      <c r="B2" s="1">
-        <v>150</v>
-      </c>
-      <c r="C2" s="1">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="1">
-        <v>150</v>
-      </c>
-      <c r="C3" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B4" s="1">
-        <v>150</v>
-      </c>
-      <c r="C4" s="1">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>1775</v>
-      </c>
-      <c r="B5" s="1">
-        <v>230</v>
-      </c>
-      <c r="C5" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>1776</v>
-      </c>
-      <c r="B6" s="1">
-        <v>300</v>
-      </c>
-      <c r="C6" s="1">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>1779</v>
-      </c>
-      <c r="B7" s="1">
-        <v>300</v>
-      </c>
-      <c r="C7" s="1">
-        <v>380</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8D45CC-6101-4FEE-B1F3-9CE1EFC50472}">
   <dimension ref="A1:K682"/>
   <sheetViews>
@@ -42620,6 +42227,400 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4407B8D6-4BCD-4778-A70E-F76356A6ED49}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B1" s="70" t="s">
+        <v>1746</v>
+      </c>
+      <c r="C1" s="70" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="70" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="70" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1793</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="70" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1791</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="70" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1792</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="70" t="s">
+        <v>1755</v>
+      </c>
+      <c r="B5">
+        <v>0.75</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="70" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B6">
+        <v>0.1</v>
+      </c>
+      <c r="C6">
+        <v>0.3</v>
+      </c>
+      <c r="D6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="70" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B7">
+        <v>0.3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1757</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="70" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="70" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B9">
+        <v>0.1</v>
+      </c>
+      <c r="C9">
+        <v>0.1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="70" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1791</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1757</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="70" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1757</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7AF96B-9516-4E8F-906F-2D6A1CFA8D27}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B4">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>1765</v>
+      </c>
+      <c r="B5">
+        <v>380</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DBE3240-1F9D-4EBB-8E6B-063E85AF465C}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B4">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B5">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B6">
+        <v>0.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D87E58B-D1A3-4FBD-9C66-ABF5F5BF1B0C}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1777</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C2" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="1">
+        <v>150</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B4" s="1">
+        <v>150</v>
+      </c>
+      <c r="C4" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B5" s="1">
+        <v>230</v>
+      </c>
+      <c r="C5" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B6" s="1">
+        <v>300</v>
+      </c>
+      <c r="C6" s="1">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B7" s="1">
+        <v>300</v>
+      </c>
+      <c r="C7" s="1">
+        <v>380</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>